<commit_message>
Graphiques Fs et Fmax et Fmin
</commit_message>
<xml_diff>
--- a/resultats_nouveaux_points.xlsx
+++ b/resultats_nouveaux_points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c6d2936775fb277a/Documents/GitHub/piano_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_2B59D2BFD300D06FC77B251159DF50F05517E85F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0D112BC-F77A-42A5-952E-5B5B7826DFD2}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="11_2B59D2BFD300D06FC77B251159DF50F05517E85F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3897B5F-336C-4AF2-9451-B1CF40A827CF}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>Dictionnaire</t>
   </si>
@@ -246,6 +246,1333 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$A$39:$A$65</c:f>
+              <c:strCache>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>Original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>fs=44100-fbas=100-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fs=1764-fbas=100-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>fs=882-fbas=100-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>fs=44100-fbas=300-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>fs=1764-fbas=300-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>fs=1470-fbas=300-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>fs=882-fbas=300-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>fs=44100-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>fs=4410-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>fs=2205-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>fs=2004-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>fs=1764-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>fs=1575-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>fs=1470-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>fs=4410-fbas=550-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>fs=44100-fbas=550-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>fs=1470-fbas=550-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>fs=44100-fbas=1000-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>fs=8820-fbas=1000-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>fs=44100-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>fs=4410-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>fs=1917-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>fs=1837-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>fs=1764-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>fs=1696-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>fs=1633-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$39:$B$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>6.3901951583852853E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2693420973232818E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0530397668685972E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.270705596409315E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2208617601924861E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.4046420350180943E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.7077093746464894E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.2907521667527817E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.6323596304806531E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.5825993606727149E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2208617601924861E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.9117329499910868E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.4046420350180943E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.1059250454483552E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8354880584265781E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.9625004826055427E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.4414343890605089E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.102628786022816E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.6825469230566074E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.6737492891444432E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.3108039706784514E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4C56-4172-A88F-90A4EC9F7FAD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="784299472"/>
+        <c:axId val="784297552"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$A$39:$A$65</c:f>
+              <c:strCache>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>Original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>fs=44100-fbas=100-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fs=1764-fbas=100-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>fs=882-fbas=100-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>fs=44100-fbas=300-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>fs=1764-fbas=300-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>fs=1470-fbas=300-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>fs=882-fbas=300-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>fs=44100-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>fs=4410-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>fs=2205-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>fs=2004-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>fs=1764-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>fs=1575-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>fs=1470-fbas=300-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>fs=4410-fbas=550-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>fs=44100-fbas=550-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>fs=1470-fbas=550-fhaut=1500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>fs=44100-fbas=1000-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>fs=8820-fbas=1000-fhaut=5000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>fs=44100-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>fs=4410-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>fs=1917-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>fs=1837-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>fs=1764-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>fs=1696-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>fs=1633-fbas=700-fhaut=3000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$39:$E$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.62409605778633648</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65020943361897099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57062852809966247</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.724760109858409</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57691367125778303</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.73798465598005702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52948218127959146</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56802005942594647</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.64213265316249701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.74929109497223245</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.57691367125778303</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.76137547649695803</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.73798465598005702</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.44704252264533351</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.40176529039937392</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.39530274009911176</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.46880808405101593</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.49701150597415633</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.55135314375877198</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.77225749349150297</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.65950478964578951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4C56-4172-A88F-90A4EC9F7FAD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="724369824"/>
+        <c:axId val="786149072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="784299472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="784297552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="784297552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="784299472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="786149072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="724369824"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="724369824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="786149072"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>459531</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>113134</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>168311</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>95464</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDBC3570-D34D-7D18-24D8-2011D07A9781}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -537,10 +1864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="66" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1070,23 +2397,23 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="3">
         <v>0.1279137382852738</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>3.6300352755696901E-3</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>1.752676197019204</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <f t="shared" si="0"/>
         <v>0.87633809850960198</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>0.1773266791093856</v>
       </c>
     </row>
@@ -1238,48 +2565,567 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="3">
         <v>0.13112560821564989</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>3.9671281269580399E-3</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
         <v>1.3984826356725171</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <f t="shared" si="0"/>
         <v>0.69924131783625854</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>0.17902382269518841</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="3">
         <v>0.11280352832224071</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>7.573961721483208E-3</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
         <v>0.803986076567765</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <f t="shared" si="0"/>
         <v>0.4019930382838825</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <v>0.35671804677301922</v>
       </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39">
+        <v>6.3901951583852853E-2</v>
+      </c>
+      <c r="C39">
+        <v>7.6610584988890014E-4</v>
+      </c>
+      <c r="D39">
+        <v>1.248192115572673</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ref="E39" si="1">D39/2</f>
+        <v>0.62409605778633648</v>
+      </c>
+      <c r="F39">
+        <v>1.537968430353851E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>5.2693420973232818E-2</v>
+      </c>
+      <c r="C40">
+        <v>9.1978565973603219E-4</v>
+      </c>
+      <c r="D40">
+        <v>1.300418867237942</v>
+      </c>
+      <c r="E40">
+        <f t="shared" ref="E40:E65" si="2">D40/2</f>
+        <v>0.65020943361897099</v>
+      </c>
+      <c r="F40">
+        <v>1.4922179974967181E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41">
+        <v>5.0530397668685972E-2</v>
+      </c>
+      <c r="C41">
+        <v>8.4041807182999096E-4</v>
+      </c>
+      <c r="D41">
+        <v>1.1412570561993249</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>0.57062852809966247</v>
+      </c>
+      <c r="F41">
+        <v>3.3303991861358448E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43">
+        <v>6.270705596409315E-2</v>
+      </c>
+      <c r="C43">
+        <v>8.5845353947184601E-4</v>
+      </c>
+      <c r="D43">
+        <v>1.449520219716818</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>0.724760109858409</v>
+      </c>
+      <c r="F43">
+        <v>2.0626712733701692E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <v>4.2208617601924861E-2</v>
+      </c>
+      <c r="C44">
+        <v>1.0720636923574551E-3</v>
+      </c>
+      <c r="D44">
+        <v>1.1538273425155661</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>0.57691367125778303</v>
+      </c>
+      <c r="F44">
+        <v>5.5805855969938024E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45">
+        <v>4.4046420350180943E-2</v>
+      </c>
+      <c r="C45">
+        <v>1.039820168748056E-3</v>
+      </c>
+      <c r="D45">
+        <v>1.475969311960114</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>0.73798465598005702</v>
+      </c>
+      <c r="F45">
+        <v>9.835768067614669E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47">
+        <v>6.7077093746464894E-2</v>
+      </c>
+      <c r="C47">
+        <v>7.6559368287058556E-4</v>
+      </c>
+      <c r="D47">
+        <v>1.0589643625591829</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>0.52948218127959146</v>
+      </c>
+      <c r="F47">
+        <v>8.6276608264192062E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48">
+        <v>5.2907521667527817E-2</v>
+      </c>
+      <c r="C48">
+        <v>1.017039862628984E-3</v>
+      </c>
+      <c r="D48">
+        <v>1.1360401188518929</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>0.56802005942594647</v>
+      </c>
+      <c r="F48">
+        <v>2.4489785724652071E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49">
+        <v>5.6323596304806531E-2</v>
+      </c>
+      <c r="C49">
+        <v>9.4389386272365468E-4</v>
+      </c>
+      <c r="D49">
+        <v>1.284265306324994</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>0.64213265316249701</v>
+      </c>
+      <c r="F49">
+        <v>8.3078643707806717E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50">
+        <v>7.5825993606727149E-2</v>
+      </c>
+      <c r="C50">
+        <v>1.3470882543092501E-3</v>
+      </c>
+      <c r="D50">
+        <v>1.4985821899444649</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>0.74929109497223245</v>
+      </c>
+      <c r="F50">
+        <v>3.7059638839764382E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51">
+        <v>4.2208617601924861E-2</v>
+      </c>
+      <c r="C51">
+        <v>1.0720636923574551E-3</v>
+      </c>
+      <c r="D51">
+        <v>1.1538273425155661</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>0.57691367125778303</v>
+      </c>
+      <c r="F51">
+        <v>5.5805855969938024E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52">
+        <v>6.9117329499910868E-2</v>
+      </c>
+      <c r="C52">
+        <v>1.089303971875371E-3</v>
+      </c>
+      <c r="D52">
+        <v>1.5227509529939161</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0.76137547649695803</v>
+      </c>
+      <c r="F52">
+        <v>1.861458238428304E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53">
+        <v>4.4046420350180943E-2</v>
+      </c>
+      <c r="C53">
+        <v>1.039820168748056E-3</v>
+      </c>
+      <c r="D53">
+        <v>1.475969311960114</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0.73798465598005702</v>
+      </c>
+      <c r="F53">
+        <v>9.835768067614669E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54">
+        <v>7.1059250454483552E-2</v>
+      </c>
+      <c r="C54">
+        <v>3.264970291425653E-3</v>
+      </c>
+      <c r="D54">
+        <v>0.89408504529066701</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0.44704252264533351</v>
+      </c>
+      <c r="F54">
+        <v>9.8895314382266925E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55">
+        <v>6.8354880584265781E-2</v>
+      </c>
+      <c r="C55">
+        <v>2.3302120563923269E-3</v>
+      </c>
+      <c r="D55">
+        <v>0.80353058079874784</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0.40176529039937392</v>
+      </c>
+      <c r="F55">
+        <v>5.8693012303184841E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57">
+        <v>8.9625004826055427E-2</v>
+      </c>
+      <c r="C57">
+        <v>1.367970973502745E-3</v>
+      </c>
+      <c r="D57">
+        <v>0.79060548019822352</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0.39530274009911176</v>
+      </c>
+      <c r="F57">
+        <v>1.470093707840423E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58">
+        <v>6.4414343890605089E-2</v>
+      </c>
+      <c r="C58">
+        <v>1.7294870041286571E-3</v>
+      </c>
+      <c r="D58">
+        <v>0.93761616810203186</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0.46880808405101593</v>
+      </c>
+      <c r="F58">
+        <v>4.5409489498093203E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59">
+        <v>7.102628786022816E-2</v>
+      </c>
+      <c r="C59">
+        <v>2.4674158039186358E-3</v>
+      </c>
+      <c r="D59">
+        <v>0.99402301194831266</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0.49701150597415633</v>
+      </c>
+      <c r="F59">
+        <v>6.0351459590789712E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60">
+        <v>7.6825469230566074E-2</v>
+      </c>
+      <c r="C60">
+        <v>3.6791397264423881E-3</v>
+      </c>
+      <c r="D60">
+        <v>1.102706287517544</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0.55135314375877198</v>
+      </c>
+      <c r="F60">
+        <v>0.1428384468121458</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62">
+        <v>8.6737492891444432E-2</v>
+      </c>
+      <c r="C62">
+        <v>5.7822708911129646E-3</v>
+      </c>
+      <c r="D62">
+        <v>1.5445149869830059</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0.77225749349150297</v>
+      </c>
+      <c r="F62">
+        <v>0.29659003814619389</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63">
+        <v>8.3108039706784514E-2</v>
+      </c>
+      <c r="C63">
+        <v>2.326410638836558E-3</v>
+      </c>
+      <c r="D63">
+        <v>1.319009579291579</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0.65950478964578951</v>
+      </c>
+      <c r="F63">
+        <v>6.0158038538175113E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>